<commit_message>
Fix login tests, add readme
</commit_message>
<xml_diff>
--- a/tests/test_data/Credentials.xlsx
+++ b/tests/test_data/Credentials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PujaChoudhary\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laury\OneDrive\Documents\Work\2023\Cassini\laurynh-cassini-ui-test\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DC9597E-A1B7-41AF-BC7D-3CBC35C5119B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80BB6E7-C2F9-4ABB-9F73-B5EF2159E6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E93A3932-5D4F-4C9C-8011-B17EB0C082F6}"/>
+    <workbookView xWindow="6308" yWindow="0" windowWidth="9322" windowHeight="13080" xr2:uid="{E93A3932-5D4F-4C9C-8011-B17EB0C082F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -52,6 +52,21 @@
   </si>
   <si>
     <t>ThirdTestLogin</t>
+  </si>
+  <si>
+    <t>testType</t>
+  </si>
+  <si>
+    <t>happyPath</t>
+  </si>
+  <si>
+    <t>errorPath</t>
+  </si>
+  <si>
+    <t>errorPath2</t>
+  </si>
+  <si>
+    <t>incorrect</t>
   </si>
 </sst>
 </file>
@@ -403,48 +418,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A0CEE8-3679-4139-A713-741C1095F6F8}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>